<commit_message>
inicio de la clase 14 sobre matplotlib
</commit_message>
<xml_diff>
--- a/classes/class_7/grupo_intro_ml.xlsx
+++ b/classes/class_7/grupo_intro_ml.xlsx
@@ -3,143 +3,128 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Listado-303020-1.xls" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="grupo_intro_ml.xls" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miAeWHUXthQaftSdrsRtvEizJcK0Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhkSJrCsv1XAtoIfKMysPECpHMEXg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t xml:space="preserve">cedula </t>
-  </si>
-  <si>
-    <t>Nombre</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t xml:space="preserve">Nombre          </t>
   </si>
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t xml:space="preserve">ALVAREZ CARRERO GERMAN JOSE </t>
+    <t xml:space="preserve">ALVAREZ CARRERO GERMAN JOSE        </t>
   </si>
   <si>
     <t>german.alvarez1@udea.edu.co</t>
   </si>
   <si>
-    <t>AMAYA ESCOBAR LILLEY DANIELA</t>
-  </si>
-  <si>
-    <t>lilley.amaya1@udea.edu.co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARANGO JARAMILLO JUAN JOSE </t>
+    <t xml:space="preserve">ARANGO JARAMILLO JUAN JOSE       </t>
   </si>
   <si>
     <t>juan.arangoj@udea.edu.co</t>
   </si>
   <si>
-    <t xml:space="preserve">BOLIVAR HIGUITA JUAN PABLO </t>
+    <t xml:space="preserve">BOLIVAR HIGUITA JUAN PABLO        </t>
   </si>
   <si>
     <t>jpablo.bolivar@udea.edu.co</t>
   </si>
   <si>
-    <t>BUITRAGO LORA VANESSA</t>
+    <t xml:space="preserve">BUITRAGO LORA VANESSA        </t>
   </si>
   <si>
     <t>vanessa.buitragol@udea.edu.co</t>
   </si>
   <si>
-    <t xml:space="preserve">CARDONA GÓMEZ ELIANA </t>
-  </si>
-  <si>
-    <t>eliana.cardonag1@udea.edu.co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CARDONA ZAPATA SIMON </t>
-  </si>
-  <si>
-    <t>simon.cardonaz@udea.edu.co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CORRALES BOHÓRQUEZ ANGEL </t>
+    <t xml:space="preserve">CORRALES BOHÓRQUEZ ANGEL        </t>
   </si>
   <si>
     <t>angel.corrales@udea.edu.co</t>
   </si>
   <si>
-    <t>GALLEGO JARAMILLO JUAN PABLO</t>
+    <t xml:space="preserve">GALLEGO JARAMILLO JUAN PABLO       </t>
   </si>
   <si>
     <t>juan.gallegoj@udea.edu.co</t>
   </si>
   <si>
-    <t>10	1001748329	GIL QUINTERO LISBETH YULIZA	lisbeth.gil@udea.edu.co</t>
-  </si>
-  <si>
-    <t>11	1000653700	GIRALDO GALLEGO ANA MARÍA	ana.giraldo15@udea.edu.co</t>
-  </si>
-  <si>
-    <t>12	1152456567	GIRALDO MENA YINIM ALBERTO	yinim.giraldo@udea.edu.co</t>
-  </si>
-  <si>
-    <t>13	1010141168	GRANADA ZAPATA SUSANA	susana.granada@udea.edu.co</t>
-  </si>
-  <si>
-    <t>14	1097403976	HERNANDEZ SUAREZ NICOLAS	nicolas.hernandez@udea.edu.co</t>
-  </si>
-  <si>
-    <t>15	1036966621	JIMÉNEZ GARCÍA MIGUEL ÁNGEL	miguel.jimenezg@udea.edu.co</t>
-  </si>
-  <si>
-    <t>16	1098823480	MARTINEZ PÉREZ PEDRO ALEJANDRO	pedro.martinez1@udea.edu.co</t>
-  </si>
-  <si>
-    <t>17	1035434122	MONTOYA GONZÁLEZ PABLO ANDRÉS	pabloa.montoya@udea.edu.co</t>
-  </si>
-  <si>
-    <t>18	1000754994	MORALES GARCÍA MANUELA	manuela.moralesg@udea.edu.co</t>
-  </si>
-  <si>
-    <t>19	1040367403	MOSQUERA PEREA JESÚS JHOVANNY	jhovanny.mosquera@udea.edu.co</t>
-  </si>
-  <si>
-    <t>20	1013346470	MURILLO ZAPATA MIGUEL ANGEL	mangel.murillo@udea.edu.co</t>
-  </si>
-  <si>
-    <t>21	1214747720	NARVAEZ MONSALVE KAROL ANDREA	karol.narvaez@udea.edu.co</t>
-  </si>
-  <si>
-    <t>22	1007813704	PULGARIN QUIROZ EMILY IVETTE	emily.pulgarinq@udea.edu.co</t>
-  </si>
-  <si>
-    <t>23	1001851542	RODRIGUEZ BARRIOS DAIRA LORENA	daira.rodriguez@udea.edu.co</t>
-  </si>
-  <si>
-    <t>24	1152225691	TORRES MERIÑO JOSE LUIS CAMILO	jluiscamilo.torres@udea.edu.co</t>
-  </si>
-  <si>
-    <t>25	1007722578	TRUJILLO VERTEL MAIRA ALEJANDRA	maira.trujillo@udea.edu.co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZAPATA VANEGAS JUAN CAMILO </t>
-  </si>
-  <si>
-    <t>juan.zapata100@udea.edu.co</t>
+    <t xml:space="preserve">GRANADA ZAPATA SUSANA       </t>
+  </si>
+  <si>
+    <t>susana.granada@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HERNANDEZ SUAREZ NICOLAS        </t>
+  </si>
+  <si>
+    <t>nicolas.hernandez@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIMÉNEZ GARCÍA MIGUEL ÁNGEL        </t>
+  </si>
+  <si>
+    <t>miguel.jimenezg@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARTINEZ PÉREZ PEDRO ALEJANDRO        </t>
+  </si>
+  <si>
+    <t>pedro.martinez1@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONTOYA GONZÁLEZ PABLO ANDRÉS        </t>
+  </si>
+  <si>
+    <t>pabloa.montoya@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MORALES GARCÍA MANUELA        </t>
+  </si>
+  <si>
+    <t>manuela.moralesg@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSQUERA PEREA JESÚS JHOVANNY        </t>
+  </si>
+  <si>
+    <t>jhovanny.mosquera@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MURILLO ZAPATA MIGUEL ANGEL        </t>
+  </si>
+  <si>
+    <t>mangel.murillo@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RODRIGUEZ BARRIOS DAIRA LORENA        </t>
+  </si>
+  <si>
+    <t>daira.rodriguez@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TORRES MERIÑO JOSE LUIS CAMILO        </t>
+  </si>
+  <si>
+    <t>jluiscamilo.torres@udea.edu.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -152,6 +137,10 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -174,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -183,6 +172,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,8 +392,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="37.86"/>
-    <col customWidth="1" min="3" max="3" width="32.29"/>
+    <col customWidth="1" min="1" max="1" width="45.86"/>
+    <col customWidth="1" min="2" max="2" width="34.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -411,111 +403,84 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>1.193092675E9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>1.152715251E9</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>1.152204969E9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>1.037657637E9</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>1.146437759E9</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <v>1.000305704E9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <v>1.000756943E9</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <v>1.152686248E9</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <v>1.035921687E9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -523,86 +488,48 @@
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2">
-        <v>1.01726625E9</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>